<commit_message>
Add example roster and TDD forms.
</commit_message>
<xml_diff>
--- a/src/main/resources/example.roster.xlsx
+++ b/src/main/resources/example.roster.xlsx
@@ -533,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,6 +652,11 @@
       </c>
       <c r="S2" s="4" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4381</v>
       </c>
     </row>
   </sheetData>

</xml_diff>